<commit_message>
Added DAC electricity intensity to CCS
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_CCST.xlsx
+++ b/SubRes_TMPL/SubRES_CCST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A253C1B-6A07-44DF-9671-345741D9A6F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE150E7F-5A73-4E8D-A13B-F847DF3C5162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="1980" windowWidth="26610" windowHeight="13740" firstSheet="2" activeTab="12" xr2:uid="{55565E65-86A1-4E53-88BE-3C00B48900A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="13" xr2:uid="{55565E65-86A1-4E53-88BE-3C00B48900A4}"/>
   </bookViews>
   <sheets>
     <sheet name="ANSv2-692-Home" sheetId="9" r:id="rId1"/>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="306">
   <si>
     <t>Comment</t>
   </si>
@@ -1186,6 +1186,42 @@
   </si>
   <si>
     <t>NH3</t>
+  </si>
+  <si>
+    <t>UPSELC</t>
+  </si>
+  <si>
+    <t>DAC DATA</t>
+  </si>
+  <si>
+    <t>Fasihi et al (2019)</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jclepro.2019.03.086</t>
+  </si>
+  <si>
+    <t>DAC energy intensity (based on Carbon Engineering Aqueous HT solution)</t>
+  </si>
+  <si>
+    <t>kWh-e/t</t>
+  </si>
+  <si>
+    <t>kWh-th/t</t>
+  </si>
+  <si>
+    <t>kWh-e/t_boiler</t>
+  </si>
+  <si>
+    <t>Net kWh-e/t</t>
+  </si>
+  <si>
+    <t>Net GJ/kt</t>
+  </si>
+  <si>
+    <t>Net PJ/kt</t>
+  </si>
+  <si>
+    <t>Net kt/PJ</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1235,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1502,6 +1538,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1715,7 +1758,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
@@ -1742,8 +1785,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1973,8 +2017,9 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="16" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="23"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="24">
     <cellStyle name="Comma 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Comma 2 2" xfId="15" xr:uid="{2D29F2AE-A72A-4F35-A2CA-2C4A01C4F113}"/>
     <cellStyle name="Comma 2 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1982,6 +2027,7 @@
     <cellStyle name="Heading 2" xfId="18" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="21" builtinId="18"/>
     <cellStyle name="Heading 4" xfId="22" builtinId="19"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Input" xfId="19" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2112,7 +2158,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2156,7 +2202,7 @@
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2244,7 +2290,7 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2288,7 +2334,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2815,7 +2861,7 @@
                   <a14:compatExt spid="_x0000_s55297"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000001D80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000001D80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2873,7 +2919,7 @@
                   <a14:compatExt spid="_x0000_s55298"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000002D80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000002D80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2931,7 +2977,7 @@
                   <a14:compatExt spid="_x0000_s55299"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000003D80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000003D80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2989,7 +3035,7 @@
                   <a14:compatExt spid="_x0000_s55300"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000004D80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000004D80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3052,7 +3098,7 @@
                   <a14:compatExt spid="_x0000_s57345"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000001E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000001E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3110,7 +3156,7 @@
                   <a14:compatExt spid="_x0000_s57346"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000002E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000002E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3168,7 +3214,7 @@
                   <a14:compatExt spid="_x0000_s57347"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000003E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000003E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3226,7 +3272,7 @@
                   <a14:compatExt spid="_x0000_s57348"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000004E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000004E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3284,7 +3330,7 @@
                   <a14:compatExt spid="_x0000_s57349"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000005E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000005E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3342,7 +3388,7 @@
                   <a14:compatExt spid="_x0000_s57350"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000006E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000006E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3400,7 +3446,7 @@
                   <a14:compatExt spid="_x0000_s57351"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000007E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000007E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3458,7 +3504,7 @@
                   <a14:compatExt spid="_x0000_s57352"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000008E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000008E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3516,7 +3562,7 @@
                   <a14:compatExt spid="_x0000_s57353"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000009E00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-000009E00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3574,7 +3620,7 @@
                   <a14:compatExt spid="_x0000_s57354"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-00000AE00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1000-00000AE00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3637,7 +3683,7 @@
                   <a14:compatExt spid="_x0000_s58369"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000001E40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000001E40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3695,7 +3741,7 @@
                   <a14:compatExt spid="_x0000_s58370"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000002E40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000002E40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3753,7 +3799,7 @@
                   <a14:compatExt spid="_x0000_s58371"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000003E40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000003E40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3811,7 +3857,7 @@
                   <a14:compatExt spid="_x0000_s58372"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000004E40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000004E40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3869,7 +3915,7 @@
                   <a14:compatExt spid="_x0000_s58373"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000005E40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000005E40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3927,7 +3973,7 @@
                   <a14:compatExt spid="_x0000_s58374"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000006E40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000006E40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3985,7 +4031,7 @@
                   <a14:compatExt spid="_x0000_s58375"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000007E40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000007E40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4043,7 +4089,7 @@
                   <a14:compatExt spid="_x0000_s58376"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000008E40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1100-000008E40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4106,7 +4152,7 @@
                   <a14:compatExt spid="_x0000_s59393"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000001E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000001E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4164,7 +4210,7 @@
                   <a14:compatExt spid="_x0000_s59394"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000002E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000002E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4222,7 +4268,7 @@
                   <a14:compatExt spid="_x0000_s59395"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000003E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000003E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4280,7 +4326,7 @@
                   <a14:compatExt spid="_x0000_s59396"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000004E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000004E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4338,7 +4384,7 @@
                   <a14:compatExt spid="_x0000_s59397"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000005E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000005E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4396,7 +4442,7 @@
                   <a14:compatExt spid="_x0000_s59398"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000006E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000006E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4454,7 +4500,7 @@
                   <a14:compatExt spid="_x0000_s59399"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000007E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000007E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4512,7 +4558,7 @@
                   <a14:compatExt spid="_x0000_s59400"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000008E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000008E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4570,7 +4616,7 @@
                   <a14:compatExt spid="_x0000_s59401"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000009E80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-000009E80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4628,7 +4674,7 @@
                   <a14:compatExt spid="_x0000_s59402"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-00000AE80000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1200-00000AE80000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4691,7 +4737,7 @@
                   <a14:compatExt spid="_x0000_s60418"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000002EC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000002EC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4749,7 +4795,7 @@
                   <a14:compatExt spid="_x0000_s60419"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000003EC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000003EC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4807,7 +4853,7 @@
                   <a14:compatExt spid="_x0000_s60420"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000004EC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000004EC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4865,7 +4911,7 @@
                   <a14:compatExt spid="_x0000_s60421"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000005EC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000005EC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4923,7 +4969,7 @@
                   <a14:compatExt spid="_x0000_s60422"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000006EC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000006EC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4981,7 +5027,7 @@
                   <a14:compatExt spid="_x0000_s60423"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000007EC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000007EC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5039,7 +5085,7 @@
                   <a14:compatExt spid="_x0000_s60424"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000008EC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000008EC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5097,7 +5143,7 @@
                   <a14:compatExt spid="_x0000_s60425"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000009EC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-000009EC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5155,7 +5201,7 @@
                   <a14:compatExt spid="_x0000_s60426"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-00000AEC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-00000AEC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5213,7 +5259,7 @@
                   <a14:compatExt spid="_x0000_s60427"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-00000BEC0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1300-00000BEC0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5276,7 +5322,7 @@
                   <a14:compatExt spid="_x0000_s61442"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000002F00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000002F00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5334,7 +5380,7 @@
                   <a14:compatExt spid="_x0000_s61443"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000003F00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000003F00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5392,7 +5438,7 @@
                   <a14:compatExt spid="_x0000_s61444"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000004F00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000004F00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5450,7 +5496,7 @@
                   <a14:compatExt spid="_x0000_s61445"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000005F00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000005F00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5508,7 +5554,7 @@
                   <a14:compatExt spid="_x0000_s61446"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000006F00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000006F00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5566,7 +5612,7 @@
                   <a14:compatExt spid="_x0000_s61447"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000007F00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000007F00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5624,7 +5670,7 @@
                   <a14:compatExt spid="_x0000_s61448"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000008F00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000008F00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5682,7 +5728,7 @@
                   <a14:compatExt spid="_x0000_s61449"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000009F00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000009F00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5745,7 +5791,7 @@
                   <a14:compatExt spid="_x0000_s62466"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-000002F40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000002F40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5803,7 +5849,7 @@
                   <a14:compatExt spid="_x0000_s62467"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-000003F40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000003F40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5861,7 +5907,7 @@
                   <a14:compatExt spid="_x0000_s62468"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-000004F40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000004F40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5919,7 +5965,7 @@
                   <a14:compatExt spid="_x0000_s62469"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-000005F40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000005F40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5977,7 +6023,7 @@
                   <a14:compatExt spid="_x0000_s62470"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-000006F40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000006F40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6035,7 +6081,7 @@
                   <a14:compatExt spid="_x0000_s62471"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-000007F40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000007F40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6093,7 +6139,7 @@
                   <a14:compatExt spid="_x0000_s62472"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-000008F40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000008F40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6151,7 +6197,7 @@
                   <a14:compatExt spid="_x0000_s62473"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-000009F40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-000009F40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6209,7 +6255,7 @@
                   <a14:compatExt spid="_x0000_s62474"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-00000AF40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-00000AF40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6267,7 +6313,7 @@
                   <a14:compatExt spid="_x0000_s62475"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1600-00000BF40000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1500-00000BF40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7689,7 +7735,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7733,7 +7779,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7777,7 +7823,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7831,7 +7877,7 @@
                   <a14:compatExt spid="_x0000_s102401"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000001900100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000001900100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7889,7 +7935,7 @@
                   <a14:compatExt spid="_x0000_s102402"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000002900100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000002900100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7947,7 +7993,7 @@
                   <a14:compatExt spid="_x0000_s102403"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000003900100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000003900100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8005,7 +8051,7 @@
                   <a14:compatExt spid="_x0000_s102404"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000004900100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000004900100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8063,7 +8109,7 @@
                   <a14:compatExt spid="_x0000_s102405"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000005900100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000005900100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8121,7 +8167,7 @@
                   <a14:compatExt spid="_x0000_s102407"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000007900100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000007900100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8179,7 +8225,7 @@
                   <a14:compatExt spid="_x0000_s102408"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000008900100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000008900100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8237,7 +8283,7 @@
                   <a14:compatExt spid="_x0000_s102409"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000009900100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0E00-000009900100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8745,52 +8791,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId5">
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate"/>
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet"/>
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8820,52 +8866,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId11">
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon"/>
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon"/>
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8935,18 +8981,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -8955,57 +9026,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9035,43 +9081,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -9080,32 +9101,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9503,7 +9549,7 @@
       <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" sqref="A1:B2"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10357,12 +10403,16 @@
         <f>Processes_BASE!D18</f>
         <v>PJ</v>
       </c>
+      <c r="E21" s="12" t="s">
+        <v>294</v>
+      </c>
       <c r="F21" s="12" t="str">
         <f>F10</f>
         <v>CO2CAPT</v>
       </c>
       <c r="H21" s="12">
-        <v>1</v>
+        <f>'Elc intensity Capture'!D50</f>
+        <v>126.926103622471</v>
       </c>
       <c r="L21" s="12">
         <f>0.6*17.94/-PMT(8.2%,M21,1,0,1)</f>
@@ -10626,7 +10676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46EBDEB0-3BFC-499F-A505-247C5567BFB7}">
   <dimension ref="C1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -10843,10 +10893,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E75994-C027-4B47-B1DC-158CC6369D7F}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11301,7 +11351,89 @@
         <v>225.30555555555551</v>
       </c>
     </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C38" s="64" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C39" s="64" t="s">
+        <v>296</v>
+      </c>
+      <c r="E39" s="115" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C41" s="64" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="64" t="s">
+        <v>299</v>
+      </c>
+      <c r="D43">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C44" s="64" t="s">
+        <v>300</v>
+      </c>
+      <c r="D44">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C45" s="64" t="s">
+        <v>301</v>
+      </c>
+      <c r="D45">
+        <f>D44/0.8</f>
+        <v>1822.5</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C47" s="64" t="s">
+        <v>302</v>
+      </c>
+      <c r="D47">
+        <f>D43+D45</f>
+        <v>2188.5</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="64" t="s">
+        <v>303</v>
+      </c>
+      <c r="D48">
+        <f>D47*3.6</f>
+        <v>7878.6</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="64" t="s">
+        <v>304</v>
+      </c>
+      <c r="D49">
+        <f>D48*0.000001</f>
+        <v>7.8785999999999995E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="64" t="s">
+        <v>305</v>
+      </c>
+      <c r="D50">
+        <f>D49^-1</f>
+        <v>126.926103622471</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E39" r:id="rId1" xr:uid="{32FB01E8-47EA-4E4B-A1A6-08F0162F52CA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11584,8 +11716,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102407" r:id="rId8" name="cmdCommName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102407" r:id="rId8" name="cmdCommName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102402" r:id="rId16" name="cmdProcName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102402" r:id="rId16" name="cmdProcName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -11604,182 +11911,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102402" r:id="rId6" name="cmdProcName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102402" r:id="rId6" name="cmdProcName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102407" r:id="rId14" name="cmdCommName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102407" r:id="rId14" name="cmdCommName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2"/>
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11928,8 +12060,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet">
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -11948,82 +12155,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets"/>
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12097,8 +12229,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -12117,232 +12474,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12406,8 +12538,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet">
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -12426,182 +12733,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12676,8 +12808,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -12696,232 +13053,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13160,8 +13292,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13180,232 +13537,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet"/>
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13482,8 +13614,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet">
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13502,182 +13809,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13763,8 +13895,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears">
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13783,232 +14140,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17911,8 +18043,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet">
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17931,32 +18088,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets"/>
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18017,18 +18149,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -18037,7 +18169,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18067,18 +18199,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit">
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -18087,7 +18219,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit"/>
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18286,18 +18418,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -18306,7 +18438,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18336,18 +18468,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -18356,7 +18488,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18432,18 +18564,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
+                <xdr:col>3</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -18452,7 +18584,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets"/>
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18482,18 +18614,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
+                <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -18502,7 +18634,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit"/>
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18559,44 +18691,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet">
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -18604,7 +18711,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1"/>
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18634,44 +18766,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter">
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -18679,7 +18786,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2"/>
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
NCAP_AFA-LO added to DAC
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_CCST.xlsx
+++ b/SubRes_TMPL/SubRES_CCST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE150E7F-5A73-4E8D-A13B-F847DF3C5162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD40ABEC-2418-49A4-8AA0-E69C4A245EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="13" xr2:uid="{55565E65-86A1-4E53-88BE-3C00B48900A4}"/>
+    <workbookView xWindow="4125" yWindow="615" windowWidth="23460" windowHeight="14985" activeTab="11" xr2:uid="{55565E65-86A1-4E53-88BE-3C00B48900A4}"/>
   </bookViews>
   <sheets>
     <sheet name="ANSv2-692-Home" sheetId="9" r:id="rId1"/>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y11" authorId="2" shapeId="0" xr:uid="{DDF791D8-DFEA-479B-80CC-930137638027}">
+    <comment ref="Z11" authorId="2" shapeId="0" xr:uid="{DDF791D8-DFEA-479B-80CC-930137638027}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -152,7 +152,7 @@
     60kwh/ton CO2 (IEA 2019)?</t>
       </text>
     </comment>
-    <comment ref="Z12" authorId="3" shapeId="0" xr:uid="{D580312E-16B7-41B7-A7FD-9FE1C37783CC}">
+    <comment ref="AA12" authorId="3" shapeId="0" xr:uid="{D580312E-16B7-41B7-A7FD-9FE1C37783CC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="307">
   <si>
     <t>Comment</t>
   </si>
@@ -1222,6 +1222,9 @@
   </si>
   <si>
     <t>Net kt/PJ</t>
+  </si>
+  <si>
+    <t>NCAP_AFA~LO</t>
   </si>
 </sst>
 </file>
@@ -2158,7 +2161,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2202,7 +2205,7 @@
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2290,7 +2293,7 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2334,7 +2337,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8690,10 +8693,10 @@
   <threadedComment ref="K4" dT="2021-04-23T15:27:01.15" personId="{B1B3113A-9AEB-4223-A956-A0CFC873B37D}" id="{2BA06302-F325-40AE-93BB-69DD146ABAA0}">
     <text>From Parsons Brinckerhoff 2013 adjusted for 2015, energy costs may already be included - so this is a bit on the conservative side</text>
   </threadedComment>
-  <threadedComment ref="Y11" dT="2021-04-23T15:05:32.63" personId="{B1B3113A-9AEB-4223-A956-A0CFC873B37D}" id="{DDF791D8-DFEA-479B-80CC-930137638027}">
+  <threadedComment ref="Z11" dT="2021-04-23T15:05:32.63" personId="{B1B3113A-9AEB-4223-A956-A0CFC873B37D}" id="{DDF791D8-DFEA-479B-80CC-930137638027}">
     <text>60kwh/ton CO2 (IEA 2019)?</text>
   </threadedComment>
-  <threadedComment ref="Z12" dT="2021-04-23T15:05:47.68" personId="{B1B3113A-9AEB-4223-A956-A0CFC873B37D}" id="{D580312E-16B7-41B7-A7FD-9FE1C37783CC}">
+  <threadedComment ref="AA12" dT="2021-04-23T15:05:47.68" personId="{B1B3113A-9AEB-4223-A956-A0CFC873B37D}" id="{D580312E-16B7-41B7-A7FD-9FE1C37783CC}">
     <text>3 GJ/ton (IEA 2019?)</text>
   </threadedComment>
   <threadedComment ref="H13" dT="2021-04-23T15:07:41.65" personId="{B1B3113A-9AEB-4223-A956-A0CFC873B37D}" id="{A20B0631-D7D0-4E92-A58C-D72A63ED73B0}">
@@ -8791,52 +8794,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="12289" r:id="rId4" name="cmdUpdate">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon"/>
+        <control shapeId="12289" r:id="rId4" name="cmdUpdate"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
+        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon"/>
+        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8866,52 +8869,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet"/>
+        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12289" r:id="rId12" name="cmdUpdate">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId13">
+        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12289" r:id="rId12" name="cmdUpdate"/>
+        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8981,43 +8984,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2">
+        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -9026,32 +9004,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet"/>
+        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="113666" r:id="rId6" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1"/>
+        <control shapeId="113666" r:id="rId6" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113667" r:id="rId8" name="cmdCommOUT">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113667" r:id="rId8" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9081,18 +9084,43 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113667" r:id="rId12" name="cmdCommOUT">
+        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -9101,57 +9129,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113667" r:id="rId12" name="cmdCommOUT"/>
+        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113666" r:id="rId14" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113666" r:id="rId14" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc"/>
+        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9543,13 +9546,13 @@
   <sheetPr codeName="Sheet30">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AI36"/>
+  <dimension ref="A1:AJ36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="6" ySplit="7" topLeftCell="V8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9566,17 +9569,15 @@
     <col min="17" max="22" width="8.5703125" style="12" customWidth="1"/>
     <col min="23" max="23" width="9.140625" style="12"/>
     <col min="24" max="24" width="11.42578125" style="12" customWidth="1"/>
-    <col min="25" max="29" width="10.7109375" style="12" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="12"/>
+    <col min="25" max="25" width="13.7109375" style="12" customWidth="1"/>
+    <col min="26" max="30" width="10.7109375" style="12" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11"/>
       <c r="B1" s="18"/>
       <c r="H1" s="40"/>
-      <c r="AD1" s="12" t="s">
-        <v>92</v>
-      </c>
       <c r="AE1" s="12" t="s">
         <v>92</v>
       </c>
@@ -9592,8 +9593,11 @@
       <c r="AI1" s="12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ1" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="H2" s="40"/>
       <c r="I2" s="40"/>
@@ -9601,9 +9605,6 @@
       <c r="K2" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="Y2" s="12" t="s">
-        <v>206</v>
-      </c>
       <c r="Z2" s="12" t="s">
         <v>206</v>
       </c>
@@ -9616,8 +9617,11 @@
       <c r="AC2" s="12" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD2" s="12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H3" s="71" t="s">
         <v>125</v>
       </c>
@@ -9665,11 +9669,11 @@
       <c r="X3" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Z3" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
@@ -9724,9 +9728,7 @@
       <c r="X4" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="Y4" s="70" t="s">
-        <v>121</v>
-      </c>
+      <c r="Y4" s="23"/>
       <c r="Z4" s="70" t="s">
         <v>121</v>
       </c>
@@ -9739,8 +9741,11 @@
       <c r="AC4" s="70" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD4" s="70" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H5" s="44" t="s">
         <v>27</v>
       </c>
@@ -9782,28 +9787,29 @@
         <f>F10</f>
         <v>CO2CAPT</v>
       </c>
-      <c r="Y5" s="12" t="str">
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="12" t="str">
         <f>E11</f>
         <v>INMELC</v>
       </c>
-      <c r="Z5" s="12" t="str">
+      <c r="AA5" s="12" t="str">
         <f>E12</f>
         <v>INMCEMTHF</v>
       </c>
-      <c r="AA5" s="12" t="str">
+      <c r="AB5" s="12" t="str">
         <f>E13</f>
         <v>IFAELC</v>
       </c>
-      <c r="AB5" s="12" t="str">
+      <c r="AC5" s="12" t="str">
         <f>E15</f>
         <v>ELCC</v>
       </c>
-      <c r="AC5" s="12" t="str">
+      <c r="AD5" s="12" t="str">
         <f>E20</f>
         <v>INMLIMTHF</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F6" s="66" t="s">
         <v>279</v>
       </c>
@@ -9836,7 +9842,7 @@
       </c>
       <c r="W6" s="42"/>
     </row>
-    <row r="7" spans="1:35" s="112" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" s="112" customFormat="1" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="113" t="s">
         <v>271</v>
       </c>
@@ -9906,28 +9912,31 @@
       <c r="X7" s="111" t="s">
         <v>120</v>
       </c>
-      <c r="Y7" s="113" t="str">
-        <f>"PRC_ACTFLO~"&amp;Y5</f>
+      <c r="Y7" s="111" t="s">
+        <v>306</v>
+      </c>
+      <c r="Z7" s="113" t="str">
+        <f>"PRC_ACTFLO~"&amp;Z5</f>
         <v>PRC_ACTFLO~INMELC</v>
       </c>
-      <c r="Z7" s="113" t="str">
-        <f t="shared" ref="Z7:AC7" si="0">"PRC_ACTFLO~"&amp;Z5</f>
+      <c r="AA7" s="113" t="str">
+        <f t="shared" ref="AA7:AD7" si="0">"PRC_ACTFLO~"&amp;AA5</f>
         <v>PRC_ACTFLO~INMCEMTHF</v>
       </c>
-      <c r="AA7" s="113" t="str">
+      <c r="AB7" s="113" t="str">
         <f t="shared" si="0"/>
         <v>PRC_ACTFLO~IFAELC</v>
       </c>
-      <c r="AB7" s="113" t="str">
+      <c r="AC7" s="113" t="str">
         <f t="shared" si="0"/>
         <v>PRC_ACTFLO~ELCC</v>
       </c>
-      <c r="AC7" s="113" t="str">
+      <c r="AD7" s="113" t="str">
         <f t="shared" si="0"/>
         <v>PRC_ACTFLO~INMLIMTHF</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="40" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" s="40" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="40" t="str">
         <f>RES!Y9</f>
         <v>XCO2Transport</v>
@@ -9962,7 +9971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="40" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" s="40" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="40" t="str">
         <f>RES!AI11</f>
         <v>UCO2STOR</v>
@@ -10005,7 +10014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="40" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" s="40" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="40" t="str">
         <f>RES!R8</f>
         <v>UCO2SPCEM</v>
@@ -10052,8 +10061,9 @@
       <c r="X10" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:35" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y10" s="35"/>
+    </row>
+    <row r="11" spans="1:36" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
@@ -10071,13 +10081,13 @@
       <c r="M11" s="69"/>
       <c r="N11" s="69"/>
       <c r="W11" s="12"/>
-      <c r="Y11" s="35">
+      <c r="Z11" s="35">
         <f>D30*3.6/1000000</f>
         <v>2.1599999999999999E-4</v>
       </c>
-      <c r="Z11" s="12"/>
-    </row>
-    <row r="12" spans="1:35" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AA11" s="12"/>
+    </row>
+    <row r="12" spans="1:36" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="E12" s="77" t="str">
         <f>RES!H2</f>
@@ -10099,12 +10109,12 @@
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
-      <c r="Z12" s="35">
+      <c r="AA12" s="35">
         <f>E30/1000</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="40" t="str">
         <f>RES!R15</f>
@@ -10155,7 +10165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="40" t="str">
         <f>RES!R22</f>
@@ -10206,7 +10216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="40" t="str">
         <f>RES!R28</f>
         <v>UPWRCO2SCRC</v>
@@ -10257,8 +10267,9 @@
       <c r="Z15" s="35"/>
       <c r="AA15" s="35"/>
       <c r="AB15" s="35"/>
-    </row>
-    <row r="16" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC15" s="35"/>
+    </row>
+    <row r="16" spans="1:36" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="40" t="str">
         <f>RES!R34</f>
         <v>UPWRCO2SCRG</v>
@@ -10309,8 +10320,9 @@
       <c r="Z16" s="35"/>
       <c r="AA16" s="35"/>
       <c r="AB16" s="35"/>
-    </row>
-    <row r="17" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC16" s="35"/>
+    </row>
+    <row r="17" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="40" t="str">
         <f>Processes_BASE!B15</f>
         <v>UPWRCO2SCD</v>
@@ -10340,8 +10352,9 @@
       <c r="Y17" s="35"/>
       <c r="Z17" s="35"/>
       <c r="AA17" s="35"/>
-    </row>
-    <row r="18" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AB17" s="35"/>
+    </row>
+    <row r="18" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="str">
         <f>RES!R40</f>
         <v>UCO2SPLIM</v>
@@ -10370,27 +10383,27 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E19" s="12" t="str">
         <f>RES!D2</f>
         <v>INMELC</v>
       </c>
-      <c r="Y19" s="12">
-        <f>Y11</f>
+      <c r="Z19" s="12">
+        <f>Z11</f>
         <v>2.1599999999999999E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E20" s="12" t="str">
         <f>RES!I2</f>
         <v>INMLIMTHF</v>
       </c>
-      <c r="AC20" s="12">
-        <f>Z12</f>
+      <c r="AD20" s="12">
+        <f>AA12</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="12" t="str">
         <f>Processes_BASE!B18</f>
         <v>UDACCO2S2</v>
@@ -10433,8 +10446,11 @@
       <c r="X21" s="35">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y21" s="35">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
         <v>289</v>
       </c>
@@ -10454,7 +10470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>92</v>
       </c>
@@ -10463,7 +10479,7 @@
       </c>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>92</v>
       </c>
@@ -10486,7 +10502,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>92</v>
       </c>
@@ -10505,7 +10521,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>92</v>
       </c>
@@ -10524,7 +10540,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>92</v>
       </c>
@@ -10549,7 +10565,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>92</v>
       </c>
@@ -10559,7 +10575,7 @@
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
     </row>
-    <row r="32" spans="1:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>92</v>
       </c>
@@ -10895,7 +10911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E75994-C027-4B47-B1DC-158CC6369D7F}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -11716,8 +11732,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1085850</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102402" r:id="rId6" name="cmdProcName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102402" r:id="rId6" name="cmdProcName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102403" r:id="rId8" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102403" r:id="rId8" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102407" r:id="rId14" name="cmdCommName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102407" r:id="rId14" name="cmdCommName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -11736,182 +11927,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102407" r:id="rId8" name="cmdCommName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102407" r:id="rId8" name="cmdCommName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102403" r:id="rId14" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102403" r:id="rId14" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102402" r:id="rId16" name="cmdProcName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102402" r:id="rId16" name="cmdProcName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1085850</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc"/>
+        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12060,8 +12076,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
@@ -12080,82 +12171,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet"/>
+        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12229,8 +12245,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>8</xdr:col>
@@ -12249,232 +12490,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears"/>
+        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12538,8 +12554,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6">
+        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>7</xdr:col>
@@ -12558,182 +12749,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet"/>
+        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12808,8 +12824,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode">
+        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>847725</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>8</xdr:col>
@@ -12828,232 +13069,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>847725</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears"/>
+        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13292,8 +13308,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet">
+        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13312,232 +13553,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears"/>
+        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13614,8 +13630,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6">
+        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>8</xdr:col>
@@ -13634,182 +13825,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet"/>
+        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13895,8 +13911,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode">
+        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>666750</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>9</xdr:col>
@@ -13915,232 +14156,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>666750</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears"/>
+        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18043,8 +18059,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
@@ -18063,32 +18104,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet"/>
+        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18149,18 +18165,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71683" r:id="rId4" name="cmdCommUnit">
+        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -18169,7 +18185,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71683" r:id="rId4" name="cmdCommUnit"/>
+        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18199,18 +18215,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="71683" r:id="rId8" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -18219,7 +18235,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="71683" r:id="rId8" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18418,18 +18434,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="80899" r:id="rId4" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -18438,7 +18454,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="80899" r:id="rId4" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18468,18 +18484,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80899" r:id="rId8" name="cmdProcUnits">
+        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -18488,7 +18504,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80899" r:id="rId8" name="cmdProcUnits"/>
+        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18564,18 +18580,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
+                <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -18584,7 +18600,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit"/>
+        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18614,18 +18630,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
+                <xdr:col>3</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -18634,7 +18650,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets"/>
+        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18691,19 +18707,44 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2">
+        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -18711,32 +18752,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90113" r:id="rId6" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90113" r:id="rId6" name="cmdAddParameter"/>
+        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18766,19 +18782,44 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1">
+        <control shapeId="90113" r:id="rId10" name="cmdAddParameter">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90113" r:id="rId10" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -18786,32 +18827,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet"/>
+        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
UDAC NCAP_ILED changed to 3, growth limits tightened
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_CCST.xlsx
+++ b/SubRes_TMPL/SubRES_CCST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD40ABEC-2418-49A4-8AA0-E69C4A245EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33B956F-5CAC-4F1E-9D09-125B45F45707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="615" windowWidth="23460" windowHeight="14985" activeTab="11" xr2:uid="{55565E65-86A1-4E53-88BE-3C00B48900A4}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="11" xr2:uid="{55565E65-86A1-4E53-88BE-3C00B48900A4}"/>
   </bookViews>
   <sheets>
     <sheet name="ANSv2-692-Home" sheetId="9" r:id="rId1"/>
@@ -2161,7 +2161,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2205,7 +2205,7 @@
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2293,7 +2293,7 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2337,7 +2337,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8794,52 +8794,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId5">
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate"/>
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet"/>
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8869,52 +8869,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId11">
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon"/>
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon"/>
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8984,18 +8984,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -9004,57 +9029,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9084,43 +9084,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -9129,32 +9104,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9549,10 +9549,10 @@
   <dimension ref="A1:AJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="V8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="Y21" sqref="Y21"/>
+      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10435,7 +10435,7 @@
         <v>25</v>
       </c>
       <c r="N21" s="12">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="V21" s="12">
         <v>-1</v>
@@ -11732,8 +11732,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102407" r:id="rId8" name="cmdCommName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102407" r:id="rId8" name="cmdCommName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102402" r:id="rId16" name="cmdProcName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102402" r:id="rId16" name="cmdProcName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -11752,182 +11927,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102402" r:id="rId6" name="cmdProcName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102402" r:id="rId6" name="cmdProcName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102407" r:id="rId14" name="cmdCommName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102407" r:id="rId14" name="cmdCommName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2"/>
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12076,8 +12076,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet">
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -12096,82 +12171,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets"/>
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12245,8 +12245,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -12265,232 +12490,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12554,8 +12554,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet">
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -12574,182 +12749,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12824,8 +12824,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -12844,232 +13069,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13308,8 +13308,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13328,232 +13553,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet"/>
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13630,8 +13630,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet">
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13650,182 +13825,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13911,8 +13911,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears">
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13931,232 +14156,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18059,8 +18059,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet">
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -18079,32 +18104,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets"/>
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18165,18 +18165,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -18185,7 +18185,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18215,18 +18215,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit">
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -18235,7 +18235,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit"/>
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18434,18 +18434,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -18454,7 +18454,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18484,18 +18484,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -18504,7 +18504,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18580,18 +18580,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
+                <xdr:col>3</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -18600,7 +18600,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets"/>
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18630,18 +18630,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
+                <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -18650,7 +18650,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit"/>
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18707,44 +18707,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet">
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -18752,7 +18727,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1"/>
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -18782,44 +18782,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter">
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -18827,7 +18802,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2"/>
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Updated costs for iron and steel CCS
It didnt get committed in the last
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_CCST.xlsx
+++ b/SubRes_TMPL/SubRES_CCST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A869999F-E200-44AF-8E00-629A440B2508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FEC02F-9A72-4599-BBE4-07AF84033699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="11" xr2:uid="{55565E65-86A1-4E53-88BE-3C00B48900A4}"/>
   </bookViews>
@@ -2669,7 +2669,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2713,7 +2713,7 @@
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2801,7 +2801,7 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2845,7 +2845,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9483,52 +9483,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId5">
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate"/>
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet"/>
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9558,52 +9558,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId11">
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon"/>
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon"/>
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9673,18 +9673,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -9693,57 +9718,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9773,43 +9773,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -9818,32 +9793,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10262,10 +10262,10 @@
   <dimension ref="A1:AK37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="R8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10968,13 +10968,16 @@
         <v>CO2CAPT</v>
       </c>
       <c r="H15" s="105">
-        <f>H14</f>
-        <v>833.33333333333337</v>
+        <f>1/('Iron and Steel'!N74/1000000*1000)</f>
+        <v>1942.5019425019423</v>
       </c>
       <c r="I15" s="78"/>
       <c r="J15" s="78"/>
       <c r="L15" s="72"/>
-      <c r="M15" s="69"/>
+      <c r="M15" s="69">
+        <f>'Storage supply curve'!G23*1.56/1000/-PMT(8.2%,N16,1,0,1)</f>
+        <v>5.4170994084550381</v>
+      </c>
       <c r="N15" s="12">
         <v>25</v>
       </c>
@@ -11686,7 +11689,7 @@
   <dimension ref="C1:T30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12725,8 +12728,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102407" r:id="rId8" name="cmdCommName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102407" r:id="rId8" name="cmdCommName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102402" r:id="rId16" name="cmdProcName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102402" r:id="rId16" name="cmdProcName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -12745,182 +12923,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102402" r:id="rId6" name="cmdProcName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102402" r:id="rId6" name="cmdProcName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102407" r:id="rId14" name="cmdCommName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102407" r:id="rId14" name="cmdCommName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2"/>
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13069,8 +13072,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet">
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13089,82 +13167,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets"/>
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13238,8 +13241,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13258,232 +13486,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13547,8 +13550,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet">
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13567,182 +13745,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13969,8 +13972,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -13989,232 +14217,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14301,8 +14304,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -14321,232 +14549,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet"/>
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14623,8 +14626,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet">
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -14643,182 +14821,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14904,8 +14907,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears">
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -14924,232 +15152,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -19348,8 +19351,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet">
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -19368,32 +19396,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets"/>
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -19454,18 +19457,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -19474,7 +19477,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -19504,18 +19507,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit">
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -19524,7 +19527,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit"/>
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -19723,18 +19726,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -19743,7 +19746,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -19773,18 +19776,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -19793,7 +19796,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -19869,18 +19872,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
+                <xdr:col>3</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -19889,7 +19892,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets"/>
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -19919,18 +19922,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
+                <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -19939,7 +19942,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit"/>
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -19996,44 +19999,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet">
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -20041,7 +20019,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1"/>
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -20071,44 +20074,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter">
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -20116,7 +20094,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2"/>
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>